<commit_message>
added overview of smells in the lego programs and remove refactoring part
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Program Name</t>
   </si>
@@ -50,79 +50,40 @@
     <t>No-op</t>
   </si>
   <si>
-    <t>Duplicated method</t>
-  </si>
-  <si>
-    <t>Unused field?</t>
-  </si>
-  <si>
-    <t>Compile-time constant</t>
-  </si>
-  <si>
-    <t>Magic number</t>
-  </si>
-  <si>
-    <t>Deprecrated method call</t>
-  </si>
-  <si>
-    <t>Missing input data</t>
-  </si>
-  <si>
-    <t>Infinite recursion</t>
-  </si>
-  <si>
-    <t>Message chain / Lasagna code</t>
-  </si>
-  <si>
-    <t>Atypical programming pattern?</t>
-  </si>
-  <si>
-    <t>Missing language features / Missing framework</t>
-  </si>
-  <si>
     <t>Long method</t>
   </si>
   <si>
-    <t>Many parameters</t>
-  </si>
-  <si>
-    <t>High conditional complexity</t>
-  </si>
-  <si>
-    <t>Inappropriate class intimacy</t>
-  </si>
-  <si>
-    <t>Method feature envy</t>
-  </si>
-  <si>
-    <t>Shotgun surgery</t>
-  </si>
-  <si>
-    <t>Nested loops</t>
-  </si>
-  <si>
-    <t>Large object state</t>
-  </si>
-  <si>
-    <t>Allocate memory inside loop</t>
-  </si>
-  <si>
-    <t>Inadequate synchronization</t>
-  </si>
-  <si>
-    <t>Intinite loop</t>
-  </si>
-  <si>
-    <t>Non-reentrant function</t>
-  </si>
-  <si>
-    <t>Only loop once</t>
-  </si>
-  <si>
-    <t>Unconnected GUI element?</t>
-  </si>
-  <si>
-    <t>No constraint on queues</t>
+    <t>Smell Name</t>
+  </si>
+  <si>
+    <t>Feature Envy</t>
+  </si>
+  <si>
+    <t>Yes, Sensor 2 is read in main program only to be fed into the my brick, would be better inside it</t>
+  </si>
+  <si>
+    <t>Inappropriate Intimacy</t>
+  </si>
+  <si>
+    <t>Lazy Class</t>
+  </si>
+  <si>
+    <t>Message Chain</t>
+  </si>
+  <si>
+    <t>Many Parameters</t>
+  </si>
+  <si>
+    <t>Duplicate Code</t>
+  </si>
+  <si>
+    <t>Dead Code</t>
+  </si>
+  <si>
+    <t>Unused Field</t>
+  </si>
+  <si>
+    <t>Use of Deprecated Interfaces</t>
   </si>
 </sst>
 </file>
@@ -457,102 +418,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17.78515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="54" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="3"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="3"/>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
added table with smells for the sumo programs, and extended related work (version from David)
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Smells per program" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
   <si>
     <t>Program Name</t>
   </si>
@@ -59,9 +60,6 @@
     <t>Feature Envy</t>
   </si>
   <si>
-    <t>Yes, Sensor 2 is read in main program only to be fed into the my brick, would be better inside it</t>
-  </si>
-  <si>
     <t>Inappropriate Intimacy</t>
   </si>
   <si>
@@ -83,7 +81,43 @@
     <t>Unused Field</t>
   </si>
   <si>
-    <t>Use of Deprecated Interfaces</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>Smell</t>
+  </si>
+  <si>
+    <t>Explanation</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Sensor 2 is read in main program only to be fed into the my block, would be better inside it</t>
+  </si>
+  <si>
+    <t>There are three my blocks with only 2 blicks inside (slaan, rij achteruit en draaien)</t>
+  </si>
+  <si>
+    <t>Long Method</t>
+  </si>
+  <si>
+    <t>Muziek block is very long, and could have been implemented with an array</t>
+  </si>
+  <si>
+    <t>Duplicated Code</t>
+  </si>
+  <si>
+    <t>The main block uses three loops, but all blocks could have been placed in parallel in 1 loop</t>
+  </si>
+  <si>
+    <t>Two blocks with the same power and direction placed consequentively, could have been merged</t>
+  </si>
+  <si>
+    <t>'draaien' is not used</t>
   </si>
 </sst>
 </file>
@@ -127,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -136,6 +170,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -151,6 +186,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>904612</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>95071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12849225" y="0"/>
+          <a:ext cx="2104762" cy="1428571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1076325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>1123487</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9389</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12687300" y="2924175"/>
+          <a:ext cx="3704762" cy="1085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -418,14 +534,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17.78515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.0703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.78515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="54" customHeight="1" x14ac:dyDescent="0.4">
@@ -439,31 +561,28 @@
         <v>8</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" t="s">
-        <v>18</v>
       </c>
       <c r="K1" t="s">
         <v>7</v>
-      </c>
-      <c r="L1" t="s">
-        <v>19</v>
       </c>
       <c r="M1" s="2"/>
       <c r="N1" s="2"/>
@@ -495,13 +614,70 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
@@ -517,14 +693,144 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>6</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.78515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added robocup to the table and started interpretation
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Smells per program" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="Smells per program" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="62">
   <si>
     <t>Program Name</t>
   </si>
@@ -118,6 +119,99 @@
   </si>
   <si>
     <t>'draaien' is not used</t>
+  </si>
+  <si>
+    <t>Weg and rij only have 1 block</t>
+  </si>
+  <si>
+    <t>Note that the rampup block was downloaded from the internet, not made by the kid himself</t>
+  </si>
+  <si>
+    <t>Variables are stored and then immediately read</t>
+  </si>
+  <si>
+    <t>Variables for the ramp are stored outside of the block, but could be in</t>
+  </si>
+  <si>
+    <t>Unused Parameter</t>
+  </si>
+  <si>
+    <t>And in the end, Rik manually set the value, so the original parameter is not used anymore</t>
+  </si>
+  <si>
+    <t>Own ramp up block is not used anymore</t>
+  </si>
+  <si>
+    <t>Tempo is defined outside of myblock, but (only) used in</t>
+  </si>
+  <si>
+    <t>Omdraaien en Rij consist of only 2 blocks</t>
+  </si>
+  <si>
+    <t>Omdraaien is not used anymore</t>
+  </si>
+  <si>
+    <t>No Op</t>
+  </si>
+  <si>
+    <t>RoboCup Nickolay</t>
+  </si>
+  <si>
+    <t>RoboCup Basic</t>
+  </si>
+  <si>
+    <t>This program did not use my blocks so is likely not to have smells</t>
+  </si>
+  <si>
+    <t>RoboCup Lijn2</t>
+  </si>
+  <si>
+    <t>Many instances here. Even a copy of a whole myblock in the code, and the two myblocks also look very common</t>
+  </si>
+  <si>
+    <t>Allebei Zwart no longer used</t>
+  </si>
+  <si>
+    <t>There is a part of the code that is bascially 'drive until yellow' but it is not in a block</t>
+  </si>
+  <si>
+    <t>The same two blocks look common (allebeizwart and allebeigroen) this is an example I explained in class</t>
+  </si>
+  <si>
+    <t>Vindhetblik is no longer used</t>
+  </si>
+  <si>
+    <t>Does not have myblocks</t>
+  </si>
+  <si>
+    <t>Because of the lack of use of my myblocks the switch blocks are quite similar.</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>S3</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>S5</t>
+  </si>
+  <si>
+    <t>S6</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
@@ -232,13 +326,13 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>257175</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>1123487</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>9389</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -258,6 +352,120 @@
         <a:xfrm>
           <a:off x="12687300" y="2924175"/>
           <a:ext cx="3704762" cy="1085714"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>811702</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1018494</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>85419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11203477" y="2019300"/>
+          <a:ext cx="3864392" cy="1733244"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>764559</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>656089</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>161446</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12375534" y="2486025"/>
+          <a:ext cx="4768330" cy="2009296"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>954978</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>837524</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>294982</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12565953" y="7762875"/>
+          <a:ext cx="3540146" cy="1533232"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -532,22 +740,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE8"/>
+  <dimension ref="A1:AE12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="17.78515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.78515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.0703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="8.78515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="54" customHeight="1" x14ac:dyDescent="0.4">
@@ -678,16 +880,82 @@
       <c r="K4" t="s">
         <v>22</v>
       </c>
+      <c r="L4" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
@@ -728,8 +996,143 @@
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
       <c r="H8" t="s">
         <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -740,10 +1143,377 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection sqref="A1:J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -796,37 +1566,199 @@
         <v>30</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C18" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B20" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C20" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added FB programs to table, updated Section 3 some more, added sizes to excel sheet
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -13,8 +13,9 @@
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Smells per program" sheetId="2" r:id="rId3"/>
+    <sheet name="Smells per program" sheetId="2" r:id="rId2"/>
+    <sheet name="Blocks per Program" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="106">
   <si>
     <t>Program Name</t>
   </si>
@@ -187,33 +188,6 @@
     <t>Because of the lack of use of my myblocks the switch blocks are quite similar.</t>
   </si>
   <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>S3</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>S6</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>R3</t>
-  </si>
-  <si>
     <t>FollowRed</t>
   </si>
   <si>
@@ -287,6 +261,90 @@
   </si>
   <si>
     <t>Betrokken 2 has an unconnected switch block</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>L4</t>
+  </si>
+  <si>
+    <t>L5</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>L7</t>
+  </si>
+  <si>
+    <t>L8</t>
+  </si>
+  <si>
+    <t>L9</t>
+  </si>
+  <si>
+    <t>L10</t>
+  </si>
+  <si>
+    <t>L11</t>
+  </si>
+  <si>
+    <t>L12</t>
+  </si>
+  <si>
+    <t>L13</t>
+  </si>
+  <si>
+    <t>L14</t>
+  </si>
+  <si>
+    <t>L15</t>
+  </si>
+  <si>
+    <t>L16</t>
+  </si>
+  <si>
+    <t>L17</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Actor</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Logic</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>MyBlocks</t>
+  </si>
+  <si>
+    <t>MyBlock Call</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>4 has over 30 blocks</t>
   </si>
 </sst>
 </file>
@@ -866,7 +924,7 @@
   <dimension ref="A1:AE21"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1260,7 +1318,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
@@ -1295,7 +1353,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>22</v>
@@ -1313,7 +1371,7 @@
         <v>22</v>
       </c>
       <c r="G15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="H15" t="s">
         <v>18</v>
@@ -1328,12 +1386,12 @@
         <v>22</v>
       </c>
       <c r="L15" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
         <v>22</v>
@@ -1368,7 +1426,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -1403,7 +1461,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
         <v>22</v>
@@ -1438,7 +1496,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -1473,7 +1531,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -1508,13 +1566,37 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
-        <v>79</v>
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+      <c r="F21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G21" t="s">
+        <v>22</v>
       </c>
       <c r="H21" t="s">
         <v>18</v>
       </c>
       <c r="I21" t="s">
         <v>18</v>
+      </c>
+      <c r="J21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K21" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1528,377 +1610,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" t="s">
-        <v>56</v>
-      </c>
-      <c r="F1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I1" t="s">
-        <v>60</v>
-      </c>
-      <c r="J1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D49"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -2148,141 +1863,1320 @@
     </row>
     <row r="31" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A31" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>15</v>
       </c>
       <c r="C35" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B37" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B39" t="s">
         <v>15</v>
       </c>
       <c r="C39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B43" t="s">
         <v>25</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B44" t="s">
         <v>16</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B45" t="s">
         <v>17</v>
       </c>
       <c r="C45" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B46" t="s">
         <v>7</v>
       </c>
       <c r="C46" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="C48" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
         <v>16</v>
       </c>
       <c r="C49" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>25</v>
+      </c>
+      <c r="C50" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>104</v>
+      </c>
+      <c r="J2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>6</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>104</v>
+      </c>
+      <c r="J3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>16</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>4</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>3</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>16</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>11</v>
+      </c>
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>6</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>11</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>15</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>15</v>
+      </c>
+      <c r="E15">
+        <v>4</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>19</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>78</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>27</v>
+      </c>
+      <c r="H18">
+        <v>13</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R11"/>
+  <sheetViews>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection sqref="A1:R11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>93</v>
+      </c>
+      <c r="R1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>18</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
+        <v>22</v>
+      </c>
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>18</v>
+      </c>
+      <c r="R8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>18</v>
+      </c>
+      <c r="P10" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s">
+        <v>18</v>
+      </c>
+      <c r="P11" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
further removed LabView, added Lego sizes to Table 2
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="107">
   <si>
     <t>Program Name</t>
   </si>
@@ -345,6 +345,9 @@
   </si>
   <si>
     <t>4 has over 30 blocks</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -2018,7 +2021,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B2" sqref="B2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -2027,6 +2030,9 @@
       <c r="A1" t="s">
         <v>95</v>
       </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
       <c r="C1" t="s">
         <v>99</v>
       </c>
@@ -2056,6 +2062,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2">
+        <f>SUM(C2:J2)</f>
+        <v>17</v>
+      </c>
       <c r="C2">
         <v>1</v>
       </c>
@@ -2085,6 +2095,10 @@
       <c r="A3" t="s">
         <v>2</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B18" si="0">SUM(C3:J3)</f>
+        <v>11</v>
+      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -2114,6 +2128,10 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="C4">
         <v>2</v>
       </c>
@@ -2143,6 +2161,10 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
       <c r="C5">
         <v>5</v>
       </c>
@@ -2172,6 +2194,10 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -2201,6 +2227,10 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -2230,6 +2260,10 @@
       <c r="A8" t="s">
         <v>45</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
       <c r="C8">
         <v>4</v>
       </c>
@@ -2259,6 +2293,10 @@
       <c r="A9" t="s">
         <v>42</v>
       </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
       <c r="C9">
         <v>4</v>
       </c>
@@ -2288,6 +2326,10 @@
       <c r="A10" t="s">
         <v>43</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="C10">
         <v>1</v>
       </c>
@@ -2317,6 +2359,10 @@
       <c r="A11" t="s">
         <v>57</v>
       </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="C11">
         <v>0</v>
       </c>
@@ -2346,6 +2392,10 @@
       <c r="A12" t="s">
         <v>53</v>
       </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="C12">
         <v>0</v>
       </c>
@@ -2375,6 +2425,10 @@
       <c r="A13" t="s">
         <v>61</v>
       </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
       <c r="C13">
         <v>2</v>
       </c>
@@ -2404,6 +2458,10 @@
       <c r="A14" t="s">
         <v>64</v>
       </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
       <c r="C14">
         <v>0</v>
       </c>
@@ -2433,6 +2491,10 @@
       <c r="A15" t="s">
         <v>69</v>
       </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
       <c r="C15">
         <v>7</v>
       </c>
@@ -2462,6 +2524,10 @@
       <c r="A16" t="s">
         <v>68</v>
       </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -2491,6 +2557,10 @@
       <c r="A17" t="s">
         <v>66</v>
       </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -2519,6 +2589,10 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>70</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>149</v>
       </c>
       <c r="C18">
         <v>0</v>

</xml_diff>

<commit_message>
updated small things in EV3 chapter, abstract and conclusions
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="106">
   <si>
     <t>Program Name</t>
   </si>
@@ -339,9 +339,6 @@
   </si>
   <si>
     <t>MyBlock Call</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>4 has over 30 blocks</t>
@@ -2007,7 +2004,7 @@
         <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2018,21 +2015,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B18"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>95</v>
       </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
       <c r="C1" t="s">
         <v>99</v>
       </c>
@@ -2057,14 +2051,13 @@
       <c r="J1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2">
-        <f>SUM(C2:J2)</f>
-        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2084,21 +2077,21 @@
       <c r="H2">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
-        <v>104</v>
-      </c>
-      <c r="J2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <f>SUM(C2:J2)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <f t="shared" ref="B3:B18" si="0">SUM(C3:J3)</f>
-        <v>11</v>
-      </c>
       <c r="C3">
         <v>0</v>
       </c>
@@ -2117,21 +2110,21 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>104</v>
-      </c>
-      <c r="J3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f>SUM(C3:J3)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
       <c r="C4">
         <v>2</v>
       </c>
@@ -2156,15 +2149,15 @@
       <c r="J4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <f>SUM(C4:J4)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
       <c r="C5">
         <v>5</v>
       </c>
@@ -2189,15 +2182,15 @@
       <c r="J5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K5">
+        <f>SUM(C5:J5)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
       <c r="C6">
         <v>0</v>
       </c>
@@ -2222,15 +2215,15 @@
       <c r="J6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <f>SUM(C6:J6)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
       <c r="C7">
         <v>0</v>
       </c>
@@ -2255,15 +2248,15 @@
       <c r="J7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K7">
+        <f>SUM(C7:J7)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>45</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>35</v>
-      </c>
       <c r="C8">
         <v>4</v>
       </c>
@@ -2288,15 +2281,15 @@
       <c r="J8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K8">
+        <f>SUM(C8:J8)</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>42</v>
       </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
       <c r="C9">
         <v>4</v>
       </c>
@@ -2321,15 +2314,15 @@
       <c r="J9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K9">
+        <f>SUM(C9:J9)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
       <c r="C10">
         <v>1</v>
       </c>
@@ -2354,15 +2347,15 @@
       <c r="J10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K10">
+        <f>SUM(C10:J10)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>57</v>
       </c>
-      <c r="B11">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
       <c r="C11">
         <v>0</v>
       </c>
@@ -2387,15 +2380,15 @@
       <c r="J11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K11">
+        <f>SUM(C11:J11)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>53</v>
       </c>
-      <c r="B12">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="C12">
         <v>0</v>
       </c>
@@ -2420,15 +2413,15 @@
       <c r="J12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K12">
+        <f>SUM(C12:J12)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>61</v>
       </c>
-      <c r="B13">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="C13">
         <v>2</v>
       </c>
@@ -2453,15 +2446,15 @@
       <c r="J13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K13">
+        <f>SUM(C13:J13)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>64</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
       <c r="C14">
         <v>0</v>
       </c>
@@ -2486,15 +2479,15 @@
       <c r="J14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K14">
+        <f>SUM(C14:J14)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>69</v>
       </c>
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
       <c r="C15">
         <v>7</v>
       </c>
@@ -2519,15 +2512,15 @@
       <c r="J15">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K15">
+        <f>SUM(C15:J15)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>68</v>
       </c>
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
       <c r="C16">
         <v>1</v>
       </c>
@@ -2552,15 +2545,15 @@
       <c r="J16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K16">
+        <f>SUM(C16:J16)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>66</v>
       </c>
-      <c r="B17">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
       <c r="C17">
         <v>1</v>
       </c>
@@ -2585,15 +2578,15 @@
       <c r="J17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="K17">
+        <f>SUM(C17:J17)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>70</v>
       </c>
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>149</v>
-      </c>
       <c r="C18">
         <v>0</v>
       </c>
@@ -2617,6 +2610,10 @@
       </c>
       <c r="J18">
         <v>6</v>
+      </c>
+      <c r="K18">
+        <f>SUM(C18:J18)</f>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2626,10 +2623,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:R11"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -3250,6 +3247,527 @@
         <v>22</v>
       </c>
     </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>5</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>2</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>7</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>1</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <v>16</v>
+      </c>
+      <c r="G14">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>10</v>
+      </c>
+      <c r="I14">
+        <v>16</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15">
+        <v>10</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <v>11</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>4</v>
+      </c>
+      <c r="N16">
+        <v>11</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>3</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17">
+        <v>4</v>
+      </c>
+      <c r="R17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
+        <v>100</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>6</v>
+      </c>
+      <c r="L18">
+        <v>6</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>15</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>7</v>
+      </c>
+      <c r="R18">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
+        <v>101</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>19</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20">
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>1</v>
+      </c>
+      <c r="Q20">
+        <v>3</v>
+      </c>
+      <c r="R20">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21">
+        <f>SUM(B13:B20)</f>
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>SUM(C13:C20)</f>
+        <v>11</v>
+      </c>
+      <c r="D21">
+        <f>SUM(D13:D20)</f>
+        <v>17</v>
+      </c>
+      <c r="E21">
+        <f>SUM(E13:E20)</f>
+        <v>26</v>
+      </c>
+      <c r="F21">
+        <f>SUM(F13:F20)</f>
+        <v>28</v>
+      </c>
+      <c r="G21">
+        <f>SUM(G13:G20)</f>
+        <v>18</v>
+      </c>
+      <c r="H21">
+        <f>SUM(H13:H20)</f>
+        <v>35</v>
+      </c>
+      <c r="I21">
+        <f>SUM(I13:I20)</f>
+        <v>50</v>
+      </c>
+      <c r="J21">
+        <f>SUM(J13:J20)</f>
+        <v>17</v>
+      </c>
+      <c r="K21">
+        <f>SUM(K13:K20)</f>
+        <v>12</v>
+      </c>
+      <c r="L21">
+        <f>SUM(L13:L20)</f>
+        <v>9</v>
+      </c>
+      <c r="M21">
+        <f>SUM(M13:M20)</f>
+        <v>10</v>
+      </c>
+      <c r="N21">
+        <f>SUM(N13:N20)</f>
+        <v>33</v>
+      </c>
+      <c r="O21">
+        <f>SUM(O13:O20)</f>
+        <v>54</v>
+      </c>
+      <c r="P21">
+        <f>SUM(P13:P20)</f>
+        <v>7</v>
+      </c>
+      <c r="Q21">
+        <f>SUM(Q13:Q20)</f>
+        <v>17</v>
+      </c>
+      <c r="R21">
+        <f>SUM(R13:R20)</f>
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added ev3 comment for Katie
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -923,7 +923,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1612,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -2084,7 +2084,7 @@
         <v>3</v>
       </c>
       <c r="K2">
-        <f>SUM(C2:J2)</f>
+        <f t="shared" ref="K2:K18" si="0">SUM(C2:J2)</f>
         <v>20</v>
       </c>
     </row>
@@ -2117,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <f>SUM(C3:J3)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
@@ -2150,7 +2150,7 @@
         <v>3</v>
       </c>
       <c r="K4">
-        <f>SUM(C4:J4)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
         <v>2</v>
       </c>
       <c r="K5">
-        <f>SUM(C5:J5)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
     </row>
@@ -2216,7 +2216,7 @@
         <v>3</v>
       </c>
       <c r="K6">
-        <f>SUM(C6:J6)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
     </row>
@@ -2249,7 +2249,7 @@
         <v>2</v>
       </c>
       <c r="K7">
-        <f>SUM(C7:J7)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
     </row>
@@ -2282,7 +2282,7 @@
         <v>2</v>
       </c>
       <c r="K8">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
@@ -2315,7 +2315,7 @@
         <v>4</v>
       </c>
       <c r="K9">
-        <f>SUM(C9:J9)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -2348,7 +2348,7 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <f>SUM(C10:J10)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
         <v>1</v>
       </c>
       <c r="K11">
-        <f>SUM(C11:J11)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -2414,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <f>SUM(C12:J12)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
     </row>
@@ -2447,7 +2447,7 @@
         <v>1</v>
       </c>
       <c r="K13">
-        <f>SUM(C13:J13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -2480,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <f>SUM(C14:J14)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -2513,7 +2513,7 @@
         <v>4</v>
       </c>
       <c r="K15">
-        <f>SUM(C15:J15)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
     </row>
@@ -2546,7 +2546,7 @@
         <v>1</v>
       </c>
       <c r="K16">
-        <f>SUM(C16:J16)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
@@ -2579,7 +2579,7 @@
         <v>3</v>
       </c>
       <c r="K17">
-        <f>SUM(C17:J17)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
     </row>
@@ -2612,7 +2612,7 @@
         <v>6</v>
       </c>
       <c r="K18">
-        <f>SUM(C18:J18)</f>
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>
@@ -2625,8 +2625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:R21"/>
+    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -3700,71 +3700,71 @@
         <v>105</v>
       </c>
       <c r="B21">
-        <f>SUM(B13:B20)</f>
+        <f t="shared" ref="B21:R21" si="0">SUM(B13:B20)</f>
         <v>20</v>
       </c>
       <c r="C21">
-        <f>SUM(C13:C20)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="D21">
-        <f>SUM(D13:D20)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="E21">
-        <f>SUM(E13:E20)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="F21">
-        <f>SUM(F13:F20)</f>
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="G21">
-        <f>SUM(G13:G20)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="H21">
-        <f>SUM(H13:H20)</f>
+        <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="I21">
-        <f>SUM(I13:I20)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="J21">
-        <f>SUM(J13:J20)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="K21">
-        <f>SUM(K13:K20)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="L21">
-        <f>SUM(L13:L20)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="M21">
-        <f>SUM(M13:M20)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="N21">
-        <f>SUM(N13:N20)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="O21">
-        <f>SUM(O13:O20)</f>
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="P21">
-        <f>SUM(P13:P20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="Q21">
-        <f>SUM(Q13:Q20)</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="R21">
-        <f>SUM(R13:R20)</f>
+        <f t="shared" si="0"/>
         <v>149</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added precentages in Section 4.1
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="14010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Smells per program" sheetId="2" r:id="rId2"/>
     <sheet name="Blocks per Program" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="Table4" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="108">
   <si>
     <t>Program Name</t>
   </si>
@@ -345,13 +345,19 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Robotics</t>
+  </si>
+  <si>
+    <t>Facebook</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="20"/>
       <color theme="1"/>
@@ -367,13 +373,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="28"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -397,7 +417,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -408,6 +428,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -1605,6 +1628,9 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <customProperties>
+    <customPr name="FormulaDeskUniqueName" r:id="rId2"/>
+  </customProperties>
 </worksheet>
 </file>
 
@@ -2623,1149 +2649,1352 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R21"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:20" ht="36" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>78</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>79</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" t="s">
         <v>81</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F2" t="s">
         <v>82</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G2" t="s">
         <v>83</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H2" t="s">
         <v>84</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I2" t="s">
         <v>85</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K2" t="s">
         <v>86</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L2" t="s">
         <v>87</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M2" t="s">
         <v>88</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N2" t="s">
         <v>89</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O2" t="s">
         <v>90</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P2" t="s">
         <v>91</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q2" t="s">
         <v>92</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R2" t="s">
         <v>93</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>22</v>
-      </c>
-      <c r="R2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" t="s">
+        <v>22</v>
+      </c>
+      <c r="L3" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" t="s">
+        <v>22</v>
+      </c>
+      <c r="O3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3">
+        <f>COUNTIF(B3:S3,"Yes")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O3" t="s">
-        <v>18</v>
-      </c>
-      <c r="P3" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>22</v>
-      </c>
-      <c r="R3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" t="s">
+        <v>22</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
+      </c>
+      <c r="O4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" t="s">
+        <v>22</v>
+      </c>
+      <c r="S4" t="s">
+        <v>22</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ref="T4:T12" si="0">COUNTIF(B4:S4,"Yes")</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" t="s">
-        <v>22</v>
-      </c>
-      <c r="L4" t="s">
-        <v>22</v>
-      </c>
-      <c r="M4" t="s">
-        <v>22</v>
-      </c>
-      <c r="N4" t="s">
-        <v>22</v>
-      </c>
-      <c r="O4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P4" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" t="s">
+        <v>22</v>
+      </c>
+      <c r="M5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>22</v>
+      </c>
+      <c r="R5" t="s">
+        <v>22</v>
+      </c>
+      <c r="S5" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" t="s">
-        <v>18</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" t="s">
-        <v>22</v>
-      </c>
-      <c r="L5" t="s">
-        <v>22</v>
-      </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5" t="s">
-        <v>22</v>
-      </c>
-      <c r="O5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>22</v>
-      </c>
-      <c r="R5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="B6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>22</v>
+      </c>
+      <c r="P6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
-        <v>22</v>
-      </c>
-      <c r="L6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N6" t="s">
-        <v>22</v>
-      </c>
-      <c r="O6" t="s">
-        <v>22</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>22</v>
-      </c>
-      <c r="R6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P7" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>22</v>
+      </c>
+      <c r="R7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S7" t="s">
+        <v>22</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
-        <v>22</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M8" t="s">
         <v>55</v>
       </c>
-      <c r="M7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="N8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>22</v>
+      </c>
+      <c r="R8" t="s">
+        <v>22</v>
+      </c>
+      <c r="S8" t="s">
+        <v>22</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" t="s">
-        <v>18</v>
-      </c>
-      <c r="L8" t="s">
-        <v>18</v>
-      </c>
-      <c r="M8" t="s">
-        <v>22</v>
-      </c>
-      <c r="N8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>18</v>
-      </c>
-      <c r="R8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="8"/>
+      <c r="K9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P9" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>22</v>
+      </c>
+      <c r="R9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" t="s">
-        <v>22</v>
-      </c>
-      <c r="L9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" t="s">
-        <v>18</v>
-      </c>
-      <c r="P9" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>22</v>
-      </c>
-      <c r="R9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>22</v>
+      </c>
+      <c r="R10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H10" t="s">
-        <v>22</v>
-      </c>
-      <c r="I10" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L10" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O10" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>22</v>
-      </c>
-      <c r="R10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R11" t="s">
+        <v>22</v>
+      </c>
+      <c r="S11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A12" t="s">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" t="s">
-        <v>22</v>
-      </c>
-      <c r="L11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N11" t="s">
-        <v>22</v>
-      </c>
-      <c r="O11" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>22</v>
-      </c>
-      <c r="R11" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>22</v>
+      </c>
+      <c r="R12" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="B14">
+        <f>COUNTIF(B3:B12,"Yes")</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:I14" si="1">COUNTIF(C3:C12,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <f>AVERAGE(B14:I14)</f>
+        <v>2.5</v>
+      </c>
+      <c r="K14">
+        <f>COUNTIF(K3:K12,"Yes")</f>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f>COUNTIF(L3:L12,"Yes")</f>
+        <v>2</v>
+      </c>
+      <c r="M14">
+        <f>COUNTIF(M3:M12,"Yes")</f>
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <f>COUNTIF(N3:N12,"Yes")</f>
+        <v>1</v>
+      </c>
+      <c r="O14">
+        <f>COUNTIF(O3:O12,"Yes")</f>
+        <v>1</v>
+      </c>
+      <c r="P14">
+        <f>COUNTIF(P3:P12,"Yes")</f>
+        <v>4</v>
+      </c>
+      <c r="Q14">
+        <f>COUNTIF(Q3:Q12,"Yes")</f>
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <f>COUNTIF(R3:R12,"Yes")</f>
+        <v>1</v>
+      </c>
+      <c r="S14">
+        <f>COUNTIF(S3:S12,"Yes")</f>
+        <v>2</v>
+      </c>
+      <c r="T14">
+        <f>AVERAGE(K14:S14)</f>
+        <v>1.4444444444444444</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>99</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17">
         <v>5</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>4</v>
       </c>
-      <c r="I13">
+      <c r="I17">
         <v>4</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="M13">
-        <v>2</v>
-      </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13">
+      <c r="J17">
+        <f t="shared" ref="J17:J23" si="2">AVERAGE(B17:I17)</f>
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
         <v>7</v>
       </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-      <c r="Q13">
-        <v>1</v>
-      </c>
-      <c r="R13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" ref="T17:T23" si="3">AVERAGE(K17:S17)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A18" t="s">
         <v>96</v>
       </c>
-      <c r="B14">
+      <c r="B18">
         <v>8</v>
       </c>
-      <c r="C14">
+      <c r="C18">
         <v>6</v>
       </c>
-      <c r="D14">
+      <c r="D18">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="E18">
         <v>7</v>
       </c>
-      <c r="F14">
+      <c r="F18">
         <v>16</v>
       </c>
-      <c r="G14">
+      <c r="G18">
         <v>8</v>
       </c>
-      <c r="H14">
+      <c r="H18">
         <v>10</v>
       </c>
-      <c r="I14">
+      <c r="I18">
         <v>16</v>
       </c>
-      <c r="J14">
+      <c r="J18">
+        <f t="shared" si="2"/>
+        <v>9.5</v>
+      </c>
+      <c r="K18">
         <v>10</v>
       </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
-      <c r="L14">
-        <v>2</v>
-      </c>
-      <c r="M14">
-        <v>1</v>
-      </c>
-      <c r="N14">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>2</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+      <c r="O18">
         <v>7</v>
       </c>
-      <c r="O14">
+      <c r="P18">
         <v>15</v>
       </c>
-      <c r="P14">
-        <v>2</v>
-      </c>
-      <c r="Q14">
-        <v>2</v>
-      </c>
-      <c r="R14">
+      <c r="Q18">
+        <v>2</v>
+      </c>
+      <c r="R18">
+        <v>2</v>
+      </c>
+      <c r="S18">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
+      <c r="T18">
+        <f t="shared" si="3"/>
+        <v>13.111111111111111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A19" t="s">
         <v>97</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>8</v>
       </c>
-      <c r="I15">
+      <c r="I19">
         <v>10</v>
       </c>
-      <c r="J15">
+      <c r="J19">
+        <f t="shared" si="2"/>
+        <v>2.75</v>
+      </c>
+      <c r="K19">
         <v>4</v>
       </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15">
-        <v>1</v>
-      </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
         <v>4</v>
       </c>
-      <c r="P15">
-        <v>2</v>
-      </c>
-      <c r="Q15">
-        <v>0</v>
-      </c>
-      <c r="R15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="Q19">
+        <v>2</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>98</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>4</v>
-      </c>
-      <c r="G16">
-        <v>3</v>
-      </c>
-      <c r="H16">
-        <v>7</v>
-      </c>
-      <c r="I16">
-        <v>11</v>
-      </c>
-      <c r="J16">
-        <v>2</v>
-      </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
-      <c r="L16">
-        <v>1</v>
-      </c>
-      <c r="M16">
-        <v>4</v>
-      </c>
-      <c r="N16">
-        <v>11</v>
-      </c>
-      <c r="O16">
-        <v>2</v>
-      </c>
-      <c r="P16">
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <v>0</v>
-      </c>
-      <c r="R16">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>103</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>2</v>
-      </c>
-      <c r="E17">
-        <v>2</v>
-      </c>
-      <c r="F17">
-        <v>3</v>
-      </c>
-      <c r="G17">
-        <v>4</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>5</v>
-      </c>
-      <c r="J17">
-        <v>0</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17">
-        <v>3</v>
-      </c>
-      <c r="P17">
-        <v>1</v>
-      </c>
-      <c r="Q17">
-        <v>4</v>
-      </c>
-      <c r="R17">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>100</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1</v>
-      </c>
-      <c r="I18">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>0</v>
-      </c>
-      <c r="K18">
-        <v>6</v>
-      </c>
-      <c r="L18">
-        <v>6</v>
-      </c>
-      <c r="M18">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>15</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <v>7</v>
-      </c>
-      <c r="R18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>0</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-      <c r="M19">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19">
-        <v>19</v>
-      </c>
-      <c r="P19">
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <v>0</v>
-      </c>
-      <c r="R19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>102</v>
       </c>
       <c r="B20">
         <v>3</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
         <v>3</v>
       </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="F20">
+      <c r="H20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>11</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="2"/>
+        <v>5.125</v>
+      </c>
+      <c r="K20">
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>4</v>
+      </c>
+      <c r="O20">
+        <v>11</v>
+      </c>
+      <c r="P20">
+        <v>2</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>25</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="3"/>
+        <v>5.2222222222222223</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21">
         <v>3</v>
       </c>
-      <c r="G20">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
-      <c r="I20">
+      <c r="G21">
         <v>4</v>
       </c>
-      <c r="J20">
-        <v>0</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>1</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
+      <c r="H21">
+        <v>3</v>
+      </c>
+      <c r="I21">
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="2"/>
+        <v>2.625</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>3</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
         <v>4</v>
       </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-      <c r="Q20">
+      <c r="S21">
+        <v>27</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="3"/>
+        <v>4.1111111111111107</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>6</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>15</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>0</v>
+      </c>
+      <c r="R22">
+        <v>7</v>
+      </c>
+      <c r="S22">
+        <v>13</v>
+      </c>
+      <c r="T22">
+        <f t="shared" si="3"/>
+        <v>5.2222222222222223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
         <v>3</v>
       </c>
-      <c r="R20">
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>19</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
+        <v>2.1111111111111112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>2</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="J24">
+        <f>AVERAGE(B24:I24)</f>
+        <v>2.375</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>1</v>
+      </c>
+      <c r="R24">
+        <v>3</v>
+      </c>
+      <c r="S24">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+      <c r="T24">
+        <f>AVERAGE(K24:S24)</f>
+        <v>1.7777777777777777</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>105</v>
       </c>
-      <c r="B21">
-        <f t="shared" ref="B21:R21" si="0">SUM(B13:B20)</f>
+      <c r="B25">
+        <f t="shared" ref="B25:I25" si="4">SUM(B17:B24)</f>
         <v>20</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
+      <c r="C25">
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
+      <c r="D25">
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
+      <c r="E25">
+        <f t="shared" si="4"/>
         <v>26</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
+      <c r="F25">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
+      <c r="G25">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
         <v>35</v>
       </c>
-      <c r="I21">
-        <f t="shared" si="0"/>
+      <c r="I25">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="0"/>
+      <c r="J25">
+        <f>MEDIAN(B25:I25)</f>
+        <v>23</v>
+      </c>
+      <c r="K25">
+        <f>SUM(K17:K24)</f>
         <v>17</v>
       </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
+      <c r="L25">
+        <f>SUM(L17:L24)</f>
         <v>12</v>
       </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
+      <c r="M25">
+        <f>SUM(M17:M24)</f>
         <v>9</v>
       </c>
-      <c r="M21">
-        <f t="shared" si="0"/>
+      <c r="N25">
+        <f>SUM(N17:N24)</f>
         <v>10</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="0"/>
+      <c r="O25">
+        <f>SUM(O17:O24)</f>
         <v>33</v>
       </c>
-      <c r="O21">
-        <f t="shared" si="0"/>
+      <c r="P25">
+        <f>SUM(P17:P24)</f>
         <v>54</v>
       </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
+      <c r="Q25">
+        <f>SUM(Q17:Q24)</f>
         <v>7</v>
       </c>
-      <c r="Q21">
-        <f t="shared" si="0"/>
+      <c r="R25">
+        <f>SUM(R17:R24)</f>
         <v>17</v>
       </c>
-      <c r="R21">
-        <f t="shared" si="0"/>
+      <c r="S25">
+        <f>SUM(S17:S24)</f>
         <v>149</v>
+      </c>
+      <c r="T25">
+        <f>MEDIAN(K25:S25)</f>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added explanation on the programs sizes and made all named exactly consistent with the EV3 IDE
</commit_message>
<xml_diff>
--- a/lego_programs.xlsx
+++ b/lego_programs.xlsx
@@ -382,18 +382,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -417,7 +411,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -429,8 +423,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2649,10 +2641,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T25"/>
+  <dimension ref="A1:S25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -2661,7 +2653,7 @@
     <col min="2" max="2" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:19" ht="36" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="6" t="s">
         <v>106</v>
       </c>
@@ -2669,7 +2661,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -2725,7 +2717,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2780,12 +2772,8 @@
       <c r="S3" t="s">
         <v>22</v>
       </c>
-      <c r="T3">
-        <f>COUNTIF(B3:S3,"Yes")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2840,12 +2828,8 @@
       <c r="S4" t="s">
         <v>22</v>
       </c>
-      <c r="T4">
-        <f t="shared" ref="T4:T12" si="0">COUNTIF(B4:S4,"Yes")</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2900,31 +2884,27 @@
       <c r="S5" t="s">
         <v>22</v>
       </c>
-      <c r="T5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
       </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" t="s">
         <v>18</v>
       </c>
       <c r="H6" t="s">
@@ -2960,12 +2940,8 @@
       <c r="S6" t="s">
         <v>22</v>
       </c>
-      <c r="T6">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -3020,12 +2996,8 @@
       <c r="S7" t="s">
         <v>22</v>
       </c>
-      <c r="T7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -3080,12 +3052,8 @@
       <c r="S8" t="s">
         <v>22</v>
       </c>
-      <c r="T8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -3098,35 +3066,34 @@
       <c r="D9" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="8"/>
-      <c r="K9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N9" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O9" s="7" t="s">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" t="s">
         <v>18</v>
       </c>
       <c r="P9" t="s">
@@ -3135,22 +3102,18 @@
       <c r="Q9" t="s">
         <v>22</v>
       </c>
-      <c r="R9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="T9">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="R9" t="s">
+        <v>18</v>
+      </c>
+      <c r="S9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10" t="s">
@@ -3159,7 +3122,7 @@
       <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" t="s">
         <v>18</v>
       </c>
       <c r="F10" t="s">
@@ -3168,10 +3131,10 @@
       <c r="G10" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="7" t="s">
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" t="s">
         <v>18</v>
       </c>
       <c r="K10" t="s">
@@ -3189,7 +3152,7 @@
       <c r="O10" t="s">
         <v>22</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" t="s">
         <v>18</v>
       </c>
       <c r="Q10" t="s">
@@ -3198,15 +3161,11 @@
       <c r="R10" t="s">
         <v>22</v>
       </c>
-      <c r="S10" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="T10">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="S10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -3261,12 +3220,8 @@
       <c r="S11" t="s">
         <v>22</v>
       </c>
-      <c r="T11">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -3321,42 +3276,38 @@
       <c r="S12" t="s">
         <v>22</v>
       </c>
-      <c r="T12">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
       <c r="B14">
         <f>COUNTIF(B3:B12,"Yes")</f>
         <v>3</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:I14" si="1">COUNTIF(C3:C12,"Yes")</f>
+        <f t="shared" ref="C14:I14" si="0">COUNTIF(C3:C12,"Yes")</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J14">
@@ -3399,12 +3350,8 @@
         <f>COUNTIF(S3:S12,"Yes")</f>
         <v>2</v>
       </c>
-      <c r="T14">
-        <f>AVERAGE(K14:S14)</f>
-        <v>1.4444444444444444</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>99</v>
       </c>
@@ -3432,10 +3379,6 @@
       <c r="I17">
         <v>4</v>
       </c>
-      <c r="J17">
-        <f t="shared" ref="J17:J23" si="2">AVERAGE(B17:I17)</f>
-        <v>2</v>
-      </c>
       <c r="K17">
         <v>1</v>
       </c>
@@ -3463,12 +3406,8 @@
       <c r="S17">
         <v>0</v>
       </c>
-      <c r="T17">
-        <f t="shared" ref="T17:T23" si="3">AVERAGE(K17:S17)</f>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>96</v>
       </c>
@@ -3496,10 +3435,6 @@
       <c r="I18">
         <v>16</v>
       </c>
-      <c r="J18">
-        <f t="shared" si="2"/>
-        <v>9.5</v>
-      </c>
       <c r="K18">
         <v>10</v>
       </c>
@@ -3527,12 +3462,8 @@
       <c r="S18">
         <v>78</v>
       </c>
-      <c r="T18">
-        <f t="shared" si="3"/>
-        <v>13.111111111111111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>97</v>
       </c>
@@ -3560,10 +3491,6 @@
       <c r="I19">
         <v>10</v>
       </c>
-      <c r="J19">
-        <f t="shared" si="2"/>
-        <v>2.75</v>
-      </c>
       <c r="K19">
         <v>4</v>
       </c>
@@ -3591,12 +3518,8 @@
       <c r="S19">
         <v>0</v>
       </c>
-      <c r="T19">
-        <f t="shared" si="3"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -3624,10 +3547,6 @@
       <c r="I20">
         <v>11</v>
       </c>
-      <c r="J20">
-        <f t="shared" si="2"/>
-        <v>5.125</v>
-      </c>
       <c r="K20">
         <v>2</v>
       </c>
@@ -3655,12 +3574,8 @@
       <c r="S20">
         <v>25</v>
       </c>
-      <c r="T20">
-        <f t="shared" si="3"/>
-        <v>5.2222222222222223</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>103</v>
       </c>
@@ -3688,10 +3603,6 @@
       <c r="I21">
         <v>5</v>
       </c>
-      <c r="J21">
-        <f t="shared" si="2"/>
-        <v>2.625</v>
-      </c>
       <c r="K21">
         <v>0</v>
       </c>
@@ -3719,12 +3630,8 @@
       <c r="S21">
         <v>27</v>
       </c>
-      <c r="T21">
-        <f t="shared" si="3"/>
-        <v>4.1111111111111107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>100</v>
       </c>
@@ -3752,10 +3659,6 @@
       <c r="I22">
         <v>0</v>
       </c>
-      <c r="J22">
-        <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
       <c r="K22">
         <v>0</v>
       </c>
@@ -3783,12 +3686,8 @@
       <c r="S22">
         <v>13</v>
       </c>
-      <c r="T22">
-        <f t="shared" si="3"/>
-        <v>5.2222222222222223</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>101</v>
       </c>
@@ -3816,10 +3715,6 @@
       <c r="I23">
         <v>0</v>
       </c>
-      <c r="J23">
-        <f t="shared" si="2"/>
-        <v>0.75</v>
-      </c>
       <c r="K23">
         <v>0</v>
       </c>
@@ -3847,12 +3742,8 @@
       <c r="S23">
         <v>0</v>
       </c>
-      <c r="T23">
-        <f t="shared" si="3"/>
-        <v>2.1111111111111112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>102</v>
       </c>
@@ -3880,10 +3771,6 @@
       <c r="I24">
         <v>4</v>
       </c>
-      <c r="J24">
-        <f>AVERAGE(B24:I24)</f>
-        <v>2.375</v>
-      </c>
       <c r="K24">
         <v>0</v>
       </c>
@@ -3911,50 +3798,42 @@
       <c r="S24">
         <v>6</v>
       </c>
-      <c r="T24">
-        <f>AVERAGE(K24:S24)</f>
-        <v>1.7777777777777777</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.4">
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>105</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:I25" si="4">SUM(B17:B24)</f>
+        <f t="shared" ref="B25:I25" si="1">SUM(B17:B24)</f>
         <v>20</v>
       </c>
       <c r="C25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="D25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="E25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="F25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="G25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="H25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>35</v>
       </c>
       <c r="I25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>50</v>
-      </c>
-      <c r="J25">
-        <f>MEDIAN(B25:I25)</f>
-        <v>23</v>
       </c>
       <c r="K25">
         <f>SUM(K17:K24)</f>
@@ -3991,10 +3870,6 @@
       <c r="S25">
         <f>SUM(S17:S24)</f>
         <v>149</v>
-      </c>
-      <c r="T25">
-        <f>MEDIAN(K25:S25)</f>
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>